<commit_message>
Report progress before meeting. Ethics and data presentation.
</commit_message>
<xml_diff>
--- a/Results Matrix.xlsx
+++ b/Results Matrix.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23120" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Demographics" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Participant</t>
   </si>
@@ -31,6 +33,48 @@
   </si>
   <si>
     <t>7-12</t>
+  </si>
+  <si>
+    <t>Q15 - Age range</t>
+  </si>
+  <si>
+    <t>18-24</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>Q16 - Occupation</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>Self-employed</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>Q17 - Frequency of Internet Usage</t>
+  </si>
+  <si>
+    <t>Multiple times per day</t>
+  </si>
+  <si>
+    <t>More than once per hour</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>S.D.</t>
   </si>
 </sst>
 </file>
@@ -62,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,12 +129,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -92,15 +164,474 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$B$17:$V$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2121295256"/>
+        <c:axId val="-2121292360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2121295256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Participant Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121292360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2121292360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Usefulness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121295256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$B$18:$V$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>3.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.666666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2120346984"/>
+        <c:axId val="-2120654424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2120346984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120654424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2120654424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120346984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>325967</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0"/>
@@ -439,12 +970,12 @@
     <col min="23" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19" customHeight="1">
+    <row r="1" spans="1:24" ht="19" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="19" customHeight="1">
+    <row r="2" spans="1:24" ht="19" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,7 +1043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="19" customHeight="1">
+    <row r="3" spans="1:24" ht="19" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -580,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="19" customHeight="1">
+    <row r="4" spans="1:24" ht="19" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -648,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="19" customHeight="1">
+    <row r="5" spans="1:24" ht="19" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -716,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="19" customHeight="1">
+    <row r="6" spans="1:24" ht="19" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -784,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="19" customHeight="1">
+    <row r="7" spans="1:24" ht="19" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -852,7 +1383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="19" customHeight="1">
+    <row r="8" spans="1:24" ht="19" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -920,7 +1451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="19" customHeight="1">
+    <row r="9" spans="1:24" ht="19" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -988,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="19" customHeight="1">
+    <row r="10" spans="1:24" ht="19" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1056,7 +1587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="19" customHeight="1">
+    <row r="11" spans="1:24" ht="19" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1124,7 +1655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="19" customHeight="1">
+    <row r="12" spans="1:24" ht="19" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1192,7 +1723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="19" customHeight="1">
+    <row r="13" spans="1:24" ht="19" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1260,7 +1791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="19" customHeight="1">
+    <row r="14" spans="1:24" ht="19" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1328,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="19" customHeight="1">
+    <row r="15" spans="1:24" ht="19" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1396,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="19" customHeight="1">
+    <row r="16" spans="1:24" ht="19" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1463,19 +1994,510 @@
       <c r="V16" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="19" customHeight="1">
+      <c r="W16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="19" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="e">
-        <f>SUM(B3:B8+B15:B16)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19" customHeight="1">
+      <c r="B17" s="1">
+        <f>AVERAGE(B3:B8,B15:B16)</f>
+        <v>3.75</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" ref="C17:V17" si="0">AVERAGE(C3:C8,C15:C16)</f>
+        <v>2.625</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.875</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.125</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.375</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.125</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.625</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.125</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.625</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.875</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="S17" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="U17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.375</v>
+      </c>
+      <c r="V17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="W17" s="1">
+        <f>AVERAGE(B17:V17)</f>
+        <v>3.5119047619047619</v>
+      </c>
+      <c r="X17" s="1">
+        <f>STDEV(B17:V17)</f>
+        <v>0.91932784711232896</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="19" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE(B9:B14)</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:V18" si="1">AVERAGE(C9:C14)</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="S18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="T18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="U18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="V18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="W18" s="1">
+        <f>AVERAGE(B18:V18)</f>
+        <v>3.4603174603174605</v>
+      </c>
+      <c r="X18" s="1">
+        <f>STDEV(B18:V18)</f>
+        <v>0.8095004665168527</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B24"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>3.875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>4.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes after meeting
</commit_message>
<xml_diff>
--- a/Results Matrix.xlsx
+++ b/Results Matrix.xlsx
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Lots of progress - added box plot, five star ratings analysis, merged results and discussion, added PCC of usefulness questions etc.
</commit_message>
<xml_diff>
--- a/Results Matrix.xlsx
+++ b/Results Matrix.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23120" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27980" windowHeight="24840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Participant</t>
   </si>
@@ -76,6 +76,18 @@
   <si>
     <t>S.D.</t>
   </si>
+  <si>
+    <t>Usefulness Questions</t>
+  </si>
+  <si>
+    <t>Usability Questions</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
 </sst>
 </file>
 
@@ -129,8 +141,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,7 +208,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -179,6 +221,21 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -191,6 +248,21 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -313,11 +385,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121295256"/>
-        <c:axId val="-2121292360"/>
+        <c:axId val="-2119961208"/>
+        <c:axId val="-2138256216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121295256"/>
+        <c:axId val="-2119961208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -345,7 +417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121292360"/>
+        <c:crossAx val="-2138256216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -353,7 +425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121292360"/>
+        <c:axId val="-2138256216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,180 +455,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121295256"/>
+        <c:crossAx val="-2119961208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:val>
-            <c:numRef>
-              <c:f>Results!$B$18:$V$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>3.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.166666666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.166666666666666</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.333333333333332</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.666666666666666</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2120346984"/>
-        <c:axId val="-2120654424"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2120346984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120654424"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2120654424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120346984"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -596,36 +499,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -956,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="V17" sqref="B17:V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0"/>
@@ -970,12 +843,12 @@
     <col min="23" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="19" customHeight="1">
+    <row r="1" spans="1:27" ht="19" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="19" customHeight="1">
+    <row r="2" spans="1:27" ht="19" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="19" customHeight="1">
+    <row r="3" spans="1:27" ht="19" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1110,8 +983,15 @@
       <c r="V3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="19" customHeight="1">
+      <c r="Z3" s="1">
+        <f>COUNTIF(B3:V8,"&gt;3") + COUNTIF(B15:V16,"&gt;3")</f>
+        <v>94</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="19" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1178,8 +1058,15 @@
       <c r="V4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="19" customHeight="1">
+      <c r="Z4" s="1">
+        <f>COUNTIF(B3:V8,"&lt;3") + COUNTIF(B15:V16,"&lt;3")</f>
+        <v>38</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="19" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1247,7 +1134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="19" customHeight="1">
+    <row r="6" spans="1:27" ht="19" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1315,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="19" customHeight="1">
+    <row r="7" spans="1:27" ht="19" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1383,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="19" customHeight="1">
+    <row r="8" spans="1:27" ht="19" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1451,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="19" customHeight="1">
+    <row r="9" spans="1:27" ht="19" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1518,8 +1405,15 @@
       <c r="V9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="19" customHeight="1">
+      <c r="Z9" s="1">
+        <f>COUNTIF(B9:V14,"&gt;3")</f>
+        <v>63</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="19" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1586,8 +1480,15 @@
       <c r="V10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="19" customHeight="1">
+      <c r="Z10" s="1">
+        <f>COUNTIF(B9:V14,"&lt;3")</f>
+        <v>30</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="19" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1655,7 +1556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="19" customHeight="1">
+    <row r="12" spans="1:27" ht="19" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1723,7 +1624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="19" customHeight="1">
+    <row r="13" spans="1:27" ht="19" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1791,7 +1692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="19" customHeight="1">
+    <row r="14" spans="1:27" ht="19" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1859,7 +1760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="19" customHeight="1">
+    <row r="15" spans="1:27" ht="19" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1927,7 +1828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="19" customHeight="1">
+    <row r="16" spans="1:27" ht="19" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2193,6 +2094,138 @@
       <c r="X18" s="1">
         <f>STDEV(B18:V18)</f>
         <v>0.8095004665168527</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="19" customHeight="1">
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <f>CORREL(B2:V2, B3:V3)</f>
+        <v>0.42441843075768043</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="19" customHeight="1">
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <f>CORREL(B2:V2, B4:V4)</f>
+        <v>0.53989547654260983</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="19" customHeight="1">
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1">
+        <f>CORREL(B2:V2, B5:V5)</f>
+        <v>0.29421006292872898</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="19" customHeight="1">
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1">
+        <f>CORREL(B2:V2, B6:V6)</f>
+        <v>0.12540958165807195</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="19" customHeight="1">
+      <c r="C41" s="1">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1">
+        <f>CORREL(B2:V2, B7:V7)</f>
+        <v>0.37091849469460791</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="19" customHeight="1">
+      <c r="C42" s="1">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1">
+        <f>CORREL(B2:V2, B8:V8)</f>
+        <v>0.42495844572108538</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="19" customHeight="1">
+      <c r="C43" s="1">
+        <v>13</v>
+      </c>
+      <c r="D43" s="1">
+        <f>CORREL(B2:V2, B15:V15)</f>
+        <v>0.61714028130003495</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="19" customHeight="1">
+      <c r="C44" s="1">
+        <v>14</v>
+      </c>
+      <c r="D44" s="1">
+        <f>CORREL(B2:V2, B16:V16)</f>
+        <v>0.23992892047822792</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="19" customHeight="1">
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1">
+        <f>CORREL(B2:V2, B9:V9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="19" customHeight="1">
+      <c r="C46" s="1">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
+        <f>CORREL(B2:V2, B10:V10)</f>
+        <v>-0.12059062967931716</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="19" customHeight="1">
+      <c r="C47" s="1">
+        <v>9</v>
+      </c>
+      <c r="D47" s="1">
+        <f>CORREL(B2:V2, B11:V11)</f>
+        <v>0.19767989419735602</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="19" customHeight="1">
+      <c r="C48" s="1">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1">
+        <f>CORREL(B2:V2, B12:V12)</f>
+        <v>0.4738941145836722</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" ht="19" customHeight="1">
+      <c r="C49" s="1">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1">
+        <f>CORREL(B2:V2, B13:V13)</f>
+        <v>5.6777870935620324E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" ht="19" customHeight="1">
+      <c r="C50" s="1">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1">
+        <f>CORREL(B2:V2, B14:V14)</f>
+        <v>2.4003840921845824E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>